<commit_message>
Download excel sheet bugs fixed
</commit_message>
<xml_diff>
--- a/public/assets/download-format/Sections_Shuffle.xlsx
+++ b/public/assets/download-format/Sections_Shuffle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ERP_K12\ERP_OLV\erp-revamp-frontend\public\assets\download-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,9 +44,6 @@
     <t>Change Subject</t>
   </si>
   <si>
-    <t>2105670678_OLVadfads</t>
-  </si>
-  <si>
     <t>[3,7]</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>[3]</t>
   </si>
   <si>
-    <t>[6,9’’]</t>
-  </si>
-  <si>
     <t>2003970002_OLV</t>
   </si>
   <si>
@@ -71,10 +65,16 @@
     <t>[23,22]</t>
   </si>
   <si>
-    <t>[70’0]</t>
-  </si>
-  <si>
     <t>[12]</t>
+  </si>
+  <si>
+    <t>2105670678_OLV</t>
+  </si>
+  <si>
+    <t>[6,9]</t>
+  </si>
+  <si>
+    <t>[700]</t>
   </si>
 </sst>
 </file>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
@@ -518,44 +518,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Section shuffling test bugs fixed
</commit_message>
<xml_diff>
--- a/public/assets/download-format/Sections_Shuffle.xlsx
+++ b/public/assets/download-format/Sections_Shuffle.xlsx
@@ -32,9 +32,6 @@
     <t>Current Grade</t>
   </si>
   <si>
-    <t>Current SectionMapping</t>
-  </si>
-  <si>
     <t>Change Grade</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>[700]</t>
+  </si>
+  <si>
+    <t>Current Section Mapping</t>
   </si>
 </sst>
 </file>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12.75"/>
@@ -506,56 +506,56 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>